<commit_message>
[6427] Segrate-shuttle en Acht-shuttle
</commit_message>
<xml_diff>
--- a/goederentreinen.xlsx
+++ b/goederentreinen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEACC05-DA56-4BF7-B2ED-40AF47882191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289CD411-B79D-402C-B58D-DCA81EFC878B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6585" yWindow="1635" windowWidth="14400" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8115" windowWidth="14400" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="161">
   <si>
     <t>Katy shuttle</t>
   </si>
@@ -508,6 +508,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=KC0oiuN_pLI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=DwPRunm3n0Y</t>
   </si>
 </sst>
 </file>
@@ -576,15 +579,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -862,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1484,82 +1479,88 @@
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A93" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B93" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Goederentreinen HSLZ standaard scenarios
</commit_message>
<xml_diff>
--- a/goederentreinen.xlsx
+++ b/goederentreinen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A80539-C403-4B3A-9436-12621B6785EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9A850D-DBF9-4645-873A-3F2B2EE4DEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8115" windowWidth="14400" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="14400" windowHeight="7484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="165">
   <si>
     <t>Katy shuttle</t>
   </si>
@@ -517,6 +517,12 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=psjqk3uLpNU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Rz1VNSCt25s</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=TE2CaAJakRs</t>
   </si>
 </sst>
 </file>
@@ -863,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1234,8 +1240,14 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -1374,8 +1386,14 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>112</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
[consist] P&O Novara shuttle
</commit_message>
<xml_diff>
--- a/goederentreinen.xlsx
+++ b/goederentreinen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9A850D-DBF9-4645-873A-3F2B2EE4DEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BF342D-713A-4B24-9B52-531013EE3F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="14400" windowHeight="7484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7380" yWindow="2640" windowWidth="14400" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="166">
   <si>
     <t>Katy shuttle</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=TE2CaAJakRs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RzhSTuUjdQI</t>
   </si>
 </sst>
 </file>
@@ -869,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1444,8 +1447,14 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+      <c r="A69" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>